<commit_message>
Add Updates to the EQG and sectors
Add Updates to the EQG and sectors
</commit_message>
<xml_diff>
--- a/Math.xlsx
+++ b/Math.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="(L-n)L^2" sheetId="1" r:id="rId1"/>
     <sheet name="sqrt(L-n)L^2" sheetId="2" r:id="rId2"/>
     <sheet name="distanceFromHighLow" sheetId="3" r:id="rId3"/>
     <sheet name="WeightedAveragedRatios" sheetId="4" r:id="rId4"/>
+    <sheet name="EQG" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Low</t>
   </si>
@@ -82,6 +83,21 @@
   <si>
     <t>WA Ratio'</t>
   </si>
+  <si>
+    <t>previous</t>
+  </si>
+  <si>
+    <t>this</t>
+  </si>
+  <si>
+    <t>this/prev</t>
+  </si>
+  <si>
+    <t>(this-prev)/max(this,prev)</t>
+  </si>
+  <si>
+    <t>(this-prev)/(abs(this)+abs(prev))</t>
+  </si>
 </sst>
 </file>
 
@@ -107,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,10 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1086,11 +1109,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="177258384"/>
-        <c:axId val="177257600"/>
+        <c:axId val="483849920"/>
+        <c:axId val="483850312"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="177258384"/>
+        <c:axId val="483849920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,12 +1170,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177257600"/>
+        <c:crossAx val="483850312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="177257600"/>
+        <c:axId val="483850312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1232,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="177258384"/>
+        <c:crossAx val="483849920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2227,11 +2250,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178342584"/>
-        <c:axId val="178344152"/>
+        <c:axId val="483855800"/>
+        <c:axId val="483849136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178342584"/>
+        <c:axId val="483855800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,12 +2311,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178344152"/>
+        <c:crossAx val="483849136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178344152"/>
+        <c:axId val="483849136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2350,7 +2373,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="178342584"/>
+        <c:crossAx val="483855800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5988,7 +6011,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -6060,7 +6083,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:F5" si="0">C3*B3</f>
+        <f t="shared" ref="D3:D5" si="0">C3*B3</f>
         <v>4</v>
       </c>
       <c r="E3">
@@ -6188,6 +6211,734 @@
       <c r="B11">
         <f>B9/B10</f>
         <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C36" si="0">IF(A2&gt;0,B2/A2-1,SIGN(B2))</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>(B2-A2)/MAX(A2,B2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>(B2-A2)/(ABS(A2)+ABS(B2))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E18" si="1">(B3-A3)/MAX(A3,B3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G18" si="2">(B3-A3)/(ABS(A3)+ABS(B3))</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>-1</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>-5</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-10</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>-1</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>-5</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>-10</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>-1</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>-5</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" t="e">
+        <f t="shared" ref="E3:E36" si="3">(B21-A21)/MAX(A21,B21)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ref="G3:G36" si="4">(B21-A21)/(ABS(A21)+ABS(B21))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>-10</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>-5</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-1.5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>-1.5</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>-5</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>-5</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>-6</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>-5</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E26" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>-1</v>
+      </c>
+      <c r="B27">
+        <v>-5</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="4"/>
+        <v>-0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>-5</v>
+      </c>
+      <c r="B28">
+        <v>-5</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>-10</v>
+      </c>
+      <c r="B29">
+        <v>-5</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>10</v>
+      </c>
+      <c r="B30">
+        <v>-10</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>-2</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>-10</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>-3</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>-10</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>-11</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>-10</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E33" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>-1</v>
+      </c>
+      <c r="B34">
+        <v>-10</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="4"/>
+        <v>-0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>-5</v>
+      </c>
+      <c r="B35">
+        <v>-10</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="4"/>
+        <v>-0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>-10</v>
+      </c>
+      <c r="B36">
+        <v>-10</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>